<commit_message>
add sprint 7 retrospective
</commit_message>
<xml_diff>
--- a/feebacks-timesheets/feedback_occurences.xlsx
+++ b/feebacks-timesheets/feedback_occurences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ed268711e0b185e/Desktop/Tesi/thesis/feebacks-timesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{ECFBA775-8208-4A57-BC95-DFC26573DE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF9F1486-6A32-47A2-9A46-9F6CF7876895}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{ECFBA775-8208-4A57-BC95-DFC26573DE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F6E7E28-B9F2-4C27-86C3-D1AF9CB7EE2B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,13 +436,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -525,10 +525,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>

</xml_diff>